<commit_message>
i like to templatize, sometimes
</commit_message>
<xml_diff>
--- a/Templates/Template.xlsx
+++ b/Templates/Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/Repository/CSV_to_ICS/Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sltcnb/Work/CSV_to_ICS/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{6B3542F0-3E95-7041-BDBB-7480AA66AE46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CBEDF26-F9CF-004D-870C-CB4866ABF040}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16320" tabRatio="823"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="28800" windowHeight="16320" tabRatio="823" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JUILLET 2020" sheetId="18" r:id="rId1"/>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="13">
-  <si>
-    <t>BEATRICE</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="12">
   <si>
     <t>27</t>
   </si>
@@ -77,11 +74,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="171" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="173" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="174" formatCode="[h]:mm"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="166" formatCode="[h]:mm"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -551,7 +548,7 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
@@ -563,7 +560,7 @@
     <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="174" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="3" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -596,19 +593,19 @@
     <xf numFmtId="20" fontId="4" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="174" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="174" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -686,16 +683,16 @@
     <xf numFmtId="20" fontId="3" fillId="6" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="4" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="174" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="174" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -731,19 +728,40 @@
     <xf numFmtId="20" fontId="3" fillId="9" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="24" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="24" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="7" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="7" fillId="0" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="24" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -755,35 +773,20 @@
     <xf numFmtId="0" fontId="8" fillId="11" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="4" fillId="0" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="4" fillId="0" borderId="18" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="4" fillId="0" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="4" fillId="0" borderId="19" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="24" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="4" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="4" fillId="0" borderId="20" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -794,66 +797,60 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="7" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="7" fillId="6" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="18" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="4" fillId="3" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="4" fillId="3" borderId="18" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="19" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="4" fillId="3" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="4" fillId="3" borderId="19" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="20" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="4" fillId="3" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="4" fillId="3" borderId="20" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="18" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="7" fillId="5" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="7" fillId="5" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="19" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="24" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="7" fillId="3" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="7" fillId="3" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="20" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="24" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Excel Built-in Normal" xfId="2"/>
+    <cellStyle name="Excel Built-in Normal" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="450">
     <dxf>
@@ -4339,14 +4336,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:W93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4356,75 +4353,75 @@
   <sheetData>
     <row r="1" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="67">
+        <v>11</v>
+      </c>
+      <c r="B1" s="88">
         <v>44011</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="67">
+      <c r="C1" s="89"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="88">
         <v>44012</v>
       </c>
-      <c r="F1" s="68"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="67">
+      <c r="F1" s="89"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="88">
         <v>44013</v>
       </c>
-      <c r="I1" s="68"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="67">
+      <c r="I1" s="89"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="88">
         <v>44014</v>
       </c>
-      <c r="L1" s="68"/>
-      <c r="M1" s="69"/>
-      <c r="N1" s="67">
+      <c r="L1" s="89"/>
+      <c r="M1" s="90"/>
+      <c r="N1" s="88">
         <v>44015</v>
       </c>
-      <c r="O1" s="68"/>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="67">
+      <c r="O1" s="89"/>
+      <c r="P1" s="90"/>
+      <c r="Q1" s="88">
         <v>44016</v>
       </c>
-      <c r="R1" s="68"/>
-      <c r="S1" s="69"/>
-      <c r="T1" s="67">
+      <c r="R1" s="89"/>
+      <c r="S1" s="90"/>
+      <c r="T1" s="88">
         <v>44017</v>
       </c>
-      <c r="U1" s="68"/>
-      <c r="V1" s="69"/>
+      <c r="U1" s="89"/>
+      <c r="V1" s="90"/>
       <c r="W1" s="15"/>
     </row>
     <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="72"/>
-      <c r="N2" s="70"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="72"/>
-      <c r="Q2" s="70"/>
-      <c r="R2" s="71"/>
-      <c r="S2" s="72"/>
-      <c r="T2" s="70"/>
-      <c r="U2" s="71"/>
-      <c r="V2" s="72"/>
+        <v>0</v>
+      </c>
+      <c r="B2" s="91"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="93"/>
+      <c r="N2" s="91"/>
+      <c r="O2" s="92"/>
+      <c r="P2" s="93"/>
+      <c r="Q2" s="91"/>
+      <c r="R2" s="92"/>
+      <c r="S2" s="93"/>
+      <c r="T2" s="91"/>
+      <c r="U2" s="92"/>
+      <c r="V2" s="93"/>
       <c r="W2" s="3"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A3" s="77" t="s">
-        <v>7</v>
+      <c r="A3" s="79" t="s">
+        <v>6</v>
       </c>
       <c r="B3" s="49">
         <v>0.59375</v>
@@ -4487,7 +4484,7 @@
       <c r="W3" s="3"/>
     </row>
     <row r="4" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="78"/>
+      <c r="A4" s="80"/>
       <c r="B4" s="51">
         <v>0.78125</v>
       </c>
@@ -4549,45 +4546,45 @@
       <c r="W4" s="3"/>
     </row>
     <row r="5" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="79"/>
-      <c r="B5" s="62"/>
-      <c r="C5" s="63"/>
+      <c r="A5" s="81"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="65"/>
       <c r="D5" s="13">
         <f>D3+D4</f>
         <v>0.25</v>
       </c>
-      <c r="E5" s="62"/>
-      <c r="F5" s="63"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="65"/>
       <c r="G5" s="13">
         <f>G3+G4</f>
         <v>0</v>
       </c>
-      <c r="H5" s="62"/>
-      <c r="I5" s="63"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="65"/>
       <c r="J5" s="13">
         <f>J4+J3</f>
         <v>0.24999999999999994</v>
       </c>
-      <c r="K5" s="62"/>
-      <c r="L5" s="63"/>
+      <c r="K5" s="64"/>
+      <c r="L5" s="65"/>
       <c r="M5" s="13">
         <f>M4+M3</f>
         <v>0.24999999999999994</v>
       </c>
-      <c r="N5" s="62"/>
-      <c r="O5" s="63"/>
+      <c r="N5" s="64"/>
+      <c r="O5" s="65"/>
       <c r="P5" s="13">
         <f>P4+P3</f>
         <v>0.24999999999999994</v>
       </c>
-      <c r="Q5" s="73"/>
-      <c r="R5" s="74"/>
+      <c r="Q5" s="59"/>
+      <c r="R5" s="60"/>
       <c r="S5" s="13">
         <f>S4+S3</f>
         <v>0</v>
       </c>
-      <c r="T5" s="73"/>
-      <c r="U5" s="74"/>
+      <c r="T5" s="59"/>
+      <c r="U5" s="60"/>
       <c r="V5" s="13">
         <f>V4+V3</f>
         <v>0</v>
@@ -4598,8 +4595,8 @@
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A6" s="59" t="s">
-        <v>8</v>
+      <c r="A6" s="76" t="s">
+        <v>7</v>
       </c>
       <c r="B6" s="20"/>
       <c r="C6" s="21"/>
@@ -4662,7 +4659,7 @@
       <c r="W6" s="3"/>
     </row>
     <row r="7" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="60"/>
+      <c r="A7" s="77"/>
       <c r="B7" s="22"/>
       <c r="C7" s="23"/>
       <c r="D7" s="10">
@@ -4709,8 +4706,8 @@
         <f>O7-N7</f>
         <v>9.375E-2</v>
       </c>
-      <c r="Q7" s="75"/>
-      <c r="R7" s="76"/>
+      <c r="Q7" s="69"/>
+      <c r="R7" s="70"/>
       <c r="S7" s="11">
         <v>0</v>
       </c>
@@ -4723,47 +4720,47 @@
       <c r="W7" s="3"/>
     </row>
     <row r="8" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="61"/>
-      <c r="B8" s="88" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="89"/>
+      <c r="A8" s="78"/>
+      <c r="B8" s="96" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="97"/>
       <c r="D8" s="13">
         <f>D6+D7</f>
         <v>0</v>
       </c>
-      <c r="E8" s="62"/>
-      <c r="F8" s="63"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="65"/>
       <c r="G8" s="13">
         <f>G6+G7</f>
         <v>0.25</v>
       </c>
-      <c r="H8" s="62"/>
-      <c r="I8" s="63"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="65"/>
       <c r="J8" s="13">
         <f>J6+J7</f>
         <v>0.25</v>
       </c>
-      <c r="K8" s="62"/>
-      <c r="L8" s="63"/>
+      <c r="K8" s="64"/>
+      <c r="L8" s="65"/>
       <c r="M8" s="13">
         <f>M6+M7</f>
         <v>0.25</v>
       </c>
-      <c r="N8" s="62"/>
-      <c r="O8" s="63"/>
+      <c r="N8" s="64"/>
+      <c r="O8" s="65"/>
       <c r="P8" s="13">
         <f>P6+P7</f>
         <v>0.25</v>
       </c>
-      <c r="Q8" s="62"/>
-      <c r="R8" s="63"/>
+      <c r="Q8" s="64"/>
+      <c r="R8" s="65"/>
       <c r="S8" s="13">
         <f>S7+S6</f>
         <v>0</v>
       </c>
-      <c r="T8" s="62"/>
-      <c r="U8" s="63"/>
+      <c r="T8" s="64"/>
+      <c r="U8" s="65"/>
       <c r="V8" s="13">
         <f>V7+V6</f>
         <v>0</v>
@@ -4774,8 +4771,8 @@
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A9" s="64" t="s">
-        <v>0</v>
+      <c r="A9" s="71" t="s">
+        <v>8</v>
       </c>
       <c r="B9" s="49">
         <v>0.32291666666666669</v>
@@ -4838,7 +4835,7 @@
       <c r="W9" s="3"/>
     </row>
     <row r="10" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="65"/>
+      <c r="A10" s="72"/>
       <c r="B10" s="51">
         <v>0.5</v>
       </c>
@@ -4900,45 +4897,45 @@
       <c r="W10" s="3"/>
     </row>
     <row r="11" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="66"/>
-      <c r="B11" s="62"/>
-      <c r="C11" s="63"/>
+      <c r="A11" s="73"/>
+      <c r="B11" s="64"/>
+      <c r="C11" s="65"/>
       <c r="D11" s="13">
         <f>D10+D9</f>
         <v>0.24999999999999994</v>
       </c>
-      <c r="E11" s="62"/>
-      <c r="F11" s="63"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="65"/>
       <c r="G11" s="13">
         <f>G10+G9</f>
         <v>0.24999999999999994</v>
       </c>
-      <c r="H11" s="62"/>
-      <c r="I11" s="63"/>
+      <c r="H11" s="64"/>
+      <c r="I11" s="65"/>
       <c r="J11" s="13">
         <f>J10+J9</f>
         <v>0</v>
       </c>
-      <c r="K11" s="62"/>
-      <c r="L11" s="63"/>
+      <c r="K11" s="64"/>
+      <c r="L11" s="65"/>
       <c r="M11" s="13">
         <f>M10+M9</f>
         <v>0</v>
       </c>
-      <c r="N11" s="93"/>
-      <c r="O11" s="94"/>
+      <c r="N11" s="74"/>
+      <c r="O11" s="75"/>
       <c r="P11" s="30">
         <f>P10+P9</f>
         <v>0</v>
       </c>
-      <c r="Q11" s="73"/>
-      <c r="R11" s="74"/>
+      <c r="Q11" s="59"/>
+      <c r="R11" s="60"/>
       <c r="S11" s="13">
         <f>S10+S9</f>
         <v>0.41666666666666669</v>
       </c>
-      <c r="T11" s="73"/>
-      <c r="U11" s="74"/>
+      <c r="T11" s="59"/>
+      <c r="U11" s="60"/>
       <c r="V11" s="13">
         <f>V10+V9</f>
         <v>0.37499999999999994</v>
@@ -4949,8 +4946,8 @@
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A12" s="90" t="s">
-        <v>10</v>
+      <c r="A12" s="66" t="s">
+        <v>9</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="5"/>
@@ -5005,7 +5002,7 @@
       <c r="W12" s="3"/>
     </row>
     <row r="13" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="91"/>
+      <c r="A13" s="67"/>
       <c r="B13" s="55">
         <v>0.60416666666666663</v>
       </c>
@@ -5070,45 +5067,45 @@
       <c r="W13" s="3"/>
     </row>
     <row r="14" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="92"/>
-      <c r="B14" s="62"/>
-      <c r="C14" s="63"/>
+      <c r="A14" s="68"/>
+      <c r="B14" s="64"/>
+      <c r="C14" s="65"/>
       <c r="D14" s="13">
         <f>D12+D13</f>
         <v>0.19791666666666674</v>
       </c>
-      <c r="E14" s="62"/>
-      <c r="F14" s="63"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="65"/>
       <c r="G14" s="13">
         <f>G13+G12</f>
         <v>0.24999999999999994</v>
       </c>
-      <c r="H14" s="62"/>
-      <c r="I14" s="63"/>
+      <c r="H14" s="64"/>
+      <c r="I14" s="65"/>
       <c r="J14" s="13">
         <f>J13+J12</f>
         <v>0.19791666666666674</v>
       </c>
-      <c r="K14" s="62"/>
-      <c r="L14" s="63"/>
+      <c r="K14" s="64"/>
+      <c r="L14" s="65"/>
       <c r="M14" s="13">
         <f>M13+M12</f>
         <v>0.19791666666666674</v>
       </c>
-      <c r="N14" s="62"/>
-      <c r="O14" s="63"/>
+      <c r="N14" s="64"/>
+      <c r="O14" s="65"/>
       <c r="P14" s="13">
         <f>P13+P12</f>
         <v>0.19791666666666674</v>
       </c>
-      <c r="Q14" s="62"/>
-      <c r="R14" s="63"/>
+      <c r="Q14" s="64"/>
+      <c r="R14" s="65"/>
       <c r="S14" s="13">
         <f>S13+S12</f>
         <v>0</v>
       </c>
-      <c r="T14" s="62"/>
-      <c r="U14" s="63"/>
+      <c r="T14" s="64"/>
+      <c r="U14" s="65"/>
       <c r="V14" s="13">
         <f>V13+V12</f>
         <v>8.3333333333333315E-2</v>
@@ -5119,8 +5116,8 @@
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A15" s="95" t="s">
-        <v>11</v>
+      <c r="A15" s="61" t="s">
+        <v>10</v>
       </c>
       <c r="B15" s="49">
         <v>0.32291666666666669</v>
@@ -5175,7 +5172,7 @@
       <c r="W15" s="3"/>
     </row>
     <row r="16" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="96"/>
+      <c r="A16" s="62"/>
       <c r="B16" s="51">
         <v>0.5</v>
       </c>
@@ -5237,45 +5234,45 @@
       <c r="W16" s="3"/>
     </row>
     <row r="17" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="97"/>
-      <c r="B17" s="62"/>
-      <c r="C17" s="63"/>
+      <c r="A17" s="63"/>
+      <c r="B17" s="64"/>
+      <c r="C17" s="65"/>
       <c r="D17" s="13">
         <f>D16+D15</f>
         <v>0.24999999999999994</v>
       </c>
-      <c r="E17" s="62"/>
-      <c r="F17" s="63"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="65"/>
       <c r="G17" s="13">
         <f>G16+G15</f>
         <v>0.19791666666666674</v>
       </c>
-      <c r="H17" s="62"/>
-      <c r="I17" s="63"/>
+      <c r="H17" s="64"/>
+      <c r="I17" s="65"/>
       <c r="J17" s="13">
         <f>J16+J15</f>
         <v>0</v>
       </c>
-      <c r="K17" s="62"/>
-      <c r="L17" s="63"/>
+      <c r="K17" s="64"/>
+      <c r="L17" s="65"/>
       <c r="M17" s="13">
         <f>M16+M15</f>
         <v>0</v>
       </c>
-      <c r="N17" s="93"/>
-      <c r="O17" s="94"/>
+      <c r="N17" s="74"/>
+      <c r="O17" s="75"/>
       <c r="P17" s="30">
         <f>P16+P15</f>
         <v>0</v>
       </c>
-      <c r="Q17" s="73"/>
-      <c r="R17" s="74"/>
+      <c r="Q17" s="59"/>
+      <c r="R17" s="60"/>
       <c r="S17" s="13">
         <f>S16+S15</f>
         <v>0.19791666666666674</v>
       </c>
-      <c r="T17" s="73"/>
-      <c r="U17" s="74"/>
+      <c r="T17" s="59"/>
+      <c r="U17" s="60"/>
       <c r="V17" s="13">
         <f>V16+V15</f>
         <v>0.28125000000000006</v>
@@ -5288,7 +5285,7 @@
     <row r="19" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="20" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B20" s="82">
         <v>44018</v>
@@ -5329,7 +5326,7 @@
     </row>
     <row r="21" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B21" s="85"/>
       <c r="C21" s="86"/>
@@ -5355,8 +5352,8 @@
       <c r="W21" s="3"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A22" s="77" t="s">
-        <v>7</v>
+      <c r="A22" s="79" t="s">
+        <v>6</v>
       </c>
       <c r="B22" s="49">
         <v>0.59375</v>
@@ -5415,7 +5412,7 @@
       <c r="W22" s="3"/>
     </row>
     <row r="23" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="78"/>
+      <c r="A23" s="80"/>
       <c r="B23" s="51">
         <v>0.78125</v>
       </c>
@@ -5458,8 +5455,8 @@
         <f>O23-N23</f>
         <v>0</v>
       </c>
-      <c r="Q23" s="75"/>
-      <c r="R23" s="76"/>
+      <c r="Q23" s="69"/>
+      <c r="R23" s="70"/>
       <c r="S23" s="11">
         <v>0</v>
       </c>
@@ -5472,45 +5469,45 @@
       <c r="W23" s="3"/>
     </row>
     <row r="24" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="79"/>
-      <c r="B24" s="62"/>
-      <c r="C24" s="63"/>
+      <c r="A24" s="81"/>
+      <c r="B24" s="64"/>
+      <c r="C24" s="65"/>
       <c r="D24" s="13">
         <f>D22+D23</f>
         <v>0.25</v>
       </c>
-      <c r="E24" s="62"/>
-      <c r="F24" s="63"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="65"/>
       <c r="G24" s="13">
         <f>G22+G23</f>
         <v>0.25</v>
       </c>
-      <c r="H24" s="62"/>
-      <c r="I24" s="63"/>
+      <c r="H24" s="64"/>
+      <c r="I24" s="65"/>
       <c r="J24" s="13">
         <f>J23+J22</f>
         <v>0.24999999999999994</v>
       </c>
-      <c r="K24" s="62"/>
-      <c r="L24" s="63"/>
+      <c r="K24" s="64"/>
+      <c r="L24" s="65"/>
       <c r="M24" s="13">
         <f>M23+M22</f>
         <v>0</v>
       </c>
-      <c r="N24" s="62"/>
-      <c r="O24" s="63"/>
+      <c r="N24" s="64"/>
+      <c r="O24" s="65"/>
       <c r="P24" s="13">
         <f>P23+P22</f>
         <v>0</v>
       </c>
-      <c r="Q24" s="62"/>
-      <c r="R24" s="63"/>
+      <c r="Q24" s="64"/>
+      <c r="R24" s="65"/>
       <c r="S24" s="13">
         <f>S23+S22</f>
         <v>0</v>
       </c>
-      <c r="T24" s="62"/>
-      <c r="U24" s="63"/>
+      <c r="T24" s="64"/>
+      <c r="U24" s="65"/>
       <c r="V24" s="13">
         <f>V23+V22</f>
         <v>0</v>
@@ -5521,8 +5518,8 @@
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A25" s="59" t="s">
-        <v>8</v>
+      <c r="A25" s="76" t="s">
+        <v>7</v>
       </c>
       <c r="B25" s="49">
         <v>0.32291666666666669</v>
@@ -5581,7 +5578,7 @@
       <c r="W25" s="3"/>
     </row>
     <row r="26" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="60"/>
+      <c r="A26" s="77"/>
       <c r="B26" s="51">
         <v>0.5</v>
       </c>
@@ -5639,45 +5636,45 @@
       <c r="W26" s="3"/>
     </row>
     <row r="27" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="61"/>
-      <c r="B27" s="62"/>
-      <c r="C27" s="63"/>
+      <c r="A27" s="78"/>
+      <c r="B27" s="64"/>
+      <c r="C27" s="65"/>
       <c r="D27" s="13">
         <f>D26+D25</f>
         <v>0.24999999999999994</v>
       </c>
-      <c r="E27" s="62"/>
-      <c r="F27" s="63"/>
+      <c r="E27" s="64"/>
+      <c r="F27" s="65"/>
       <c r="G27" s="13">
         <f>G26+G25</f>
         <v>0</v>
       </c>
-      <c r="H27" s="62"/>
-      <c r="I27" s="63"/>
+      <c r="H27" s="64"/>
+      <c r="I27" s="65"/>
       <c r="J27" s="13">
         <f>J26+J25</f>
         <v>0</v>
       </c>
-      <c r="K27" s="62"/>
-      <c r="L27" s="63"/>
+      <c r="K27" s="64"/>
+      <c r="L27" s="65"/>
       <c r="M27" s="13">
         <f>M26+M25</f>
         <v>0</v>
       </c>
-      <c r="N27" s="62"/>
-      <c r="O27" s="63"/>
+      <c r="N27" s="64"/>
+      <c r="O27" s="65"/>
       <c r="P27" s="13">
         <f>P26+P25</f>
         <v>0</v>
       </c>
-      <c r="Q27" s="73"/>
-      <c r="R27" s="74"/>
+      <c r="Q27" s="59"/>
+      <c r="R27" s="60"/>
       <c r="S27" s="13">
         <f>S26+S25</f>
         <v>0.41666666666666669</v>
       </c>
-      <c r="T27" s="73"/>
-      <c r="U27" s="74"/>
+      <c r="T27" s="59"/>
+      <c r="U27" s="60"/>
       <c r="V27" s="13">
         <f>V26+V25</f>
         <v>0.25</v>
@@ -5688,8 +5685,8 @@
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A28" s="64" t="s">
-        <v>9</v>
+      <c r="A28" s="71" t="s">
+        <v>8</v>
       </c>
       <c r="B28" s="24"/>
       <c r="C28" s="25"/>
@@ -5748,7 +5745,7 @@
       <c r="W28" s="3"/>
     </row>
     <row r="29" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="65"/>
+      <c r="A29" s="72"/>
       <c r="B29" s="27"/>
       <c r="C29" s="28"/>
       <c r="D29" s="29">
@@ -5806,45 +5803,45 @@
       <c r="W29" s="3"/>
     </row>
     <row r="30" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="66"/>
-      <c r="B30" s="93"/>
-      <c r="C30" s="94"/>
+      <c r="A30" s="73"/>
+      <c r="B30" s="74"/>
+      <c r="C30" s="75"/>
       <c r="D30" s="30">
         <f>D29+D28</f>
         <v>0</v>
       </c>
-      <c r="E30" s="62"/>
-      <c r="F30" s="63"/>
+      <c r="E30" s="64"/>
+      <c r="F30" s="65"/>
       <c r="G30" s="13">
         <f>G29+G28</f>
         <v>0.24999999999999994</v>
       </c>
-      <c r="H30" s="93"/>
-      <c r="I30" s="94"/>
+      <c r="H30" s="74"/>
+      <c r="I30" s="75"/>
       <c r="J30" s="30">
         <f>J29+J28</f>
         <v>0</v>
       </c>
-      <c r="K30" s="62"/>
-      <c r="L30" s="63"/>
+      <c r="K30" s="64"/>
+      <c r="L30" s="65"/>
       <c r="M30" s="13">
         <f>M29+M28</f>
         <v>0.24999999999999994</v>
       </c>
-      <c r="N30" s="62"/>
-      <c r="O30" s="63"/>
+      <c r="N30" s="64"/>
+      <c r="O30" s="65"/>
       <c r="P30" s="13">
         <f>P29+P28</f>
         <v>0.24999999999999994</v>
       </c>
-      <c r="Q30" s="93"/>
-      <c r="R30" s="94"/>
+      <c r="Q30" s="74"/>
+      <c r="R30" s="75"/>
       <c r="S30" s="30">
         <f>S29+S28</f>
         <v>0</v>
       </c>
-      <c r="T30" s="93"/>
-      <c r="U30" s="94"/>
+      <c r="T30" s="74"/>
+      <c r="U30" s="75"/>
       <c r="V30" s="30">
         <f>V29+V28</f>
         <v>0</v>
@@ -5855,8 +5852,8 @@
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A31" s="90" t="s">
-        <v>10</v>
+      <c r="A31" s="66" t="s">
+        <v>9</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="5"/>
@@ -5915,7 +5912,7 @@
       <c r="W31" s="46"/>
     </row>
     <row r="32" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="91"/>
+      <c r="A32" s="67"/>
       <c r="B32" s="8"/>
       <c r="C32" s="9"/>
       <c r="D32" s="10">
@@ -5977,45 +5974,45 @@
       <c r="W32" s="46"/>
     </row>
     <row r="33" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="92"/>
-      <c r="B33" s="62"/>
-      <c r="C33" s="63"/>
+      <c r="A33" s="68"/>
+      <c r="B33" s="64"/>
+      <c r="C33" s="65"/>
       <c r="D33" s="13">
         <f>D32+D31</f>
         <v>0</v>
       </c>
-      <c r="E33" s="62"/>
-      <c r="F33" s="63"/>
+      <c r="E33" s="64"/>
+      <c r="F33" s="65"/>
       <c r="G33" s="13">
         <f>G31+G32</f>
         <v>0.19791666666666674</v>
       </c>
-      <c r="H33" s="62"/>
-      <c r="I33" s="63"/>
+      <c r="H33" s="64"/>
+      <c r="I33" s="65"/>
       <c r="J33" s="13">
         <f>J31+J32</f>
         <v>0.25</v>
       </c>
-      <c r="K33" s="62"/>
-      <c r="L33" s="63"/>
+      <c r="K33" s="64"/>
+      <c r="L33" s="65"/>
       <c r="M33" s="13">
         <f>M31+M32</f>
         <v>0.25</v>
       </c>
-      <c r="N33" s="62"/>
-      <c r="O33" s="63"/>
+      <c r="N33" s="64"/>
+      <c r="O33" s="65"/>
       <c r="P33" s="13">
         <f>P31+P32</f>
         <v>0.25</v>
       </c>
-      <c r="Q33" s="73"/>
-      <c r="R33" s="74"/>
+      <c r="Q33" s="59"/>
+      <c r="R33" s="60"/>
       <c r="S33" s="13">
         <f>S32+S31</f>
         <v>0</v>
       </c>
-      <c r="T33" s="73"/>
-      <c r="U33" s="74"/>
+      <c r="T33" s="59"/>
+      <c r="U33" s="60"/>
       <c r="V33" s="13">
         <f>V32+V31</f>
         <v>0</v>
@@ -6026,8 +6023,8 @@
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A34" s="95" t="s">
-        <v>11</v>
+      <c r="A34" s="61" t="s">
+        <v>10</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="5"/>
@@ -6075,7 +6072,7 @@
       <c r="W34" s="3"/>
     </row>
     <row r="35" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="96"/>
+      <c r="A35" s="62"/>
       <c r="B35" s="55">
         <v>0.60416666666666663</v>
       </c>
@@ -6145,45 +6142,45 @@
       <c r="W35" s="3"/>
     </row>
     <row r="36" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="97"/>
-      <c r="B36" s="62"/>
-      <c r="C36" s="63"/>
+      <c r="A36" s="63"/>
+      <c r="B36" s="64"/>
+      <c r="C36" s="65"/>
       <c r="D36" s="13">
         <f>D34+D35</f>
         <v>0.19791666666666674</v>
       </c>
-      <c r="E36" s="62"/>
-      <c r="F36" s="63"/>
+      <c r="E36" s="64"/>
+      <c r="F36" s="65"/>
       <c r="G36" s="13">
         <f>G35+G34</f>
         <v>0</v>
       </c>
-      <c r="H36" s="62"/>
-      <c r="I36" s="63"/>
+      <c r="H36" s="64"/>
+      <c r="I36" s="65"/>
       <c r="J36" s="13">
         <f>J35+J34</f>
         <v>0.19791666666666674</v>
       </c>
-      <c r="K36" s="62"/>
-      <c r="L36" s="63"/>
+      <c r="K36" s="64"/>
+      <c r="L36" s="65"/>
       <c r="M36" s="13">
         <f>M35+M34</f>
         <v>0.19791666666666674</v>
       </c>
-      <c r="N36" s="62"/>
-      <c r="O36" s="63"/>
+      <c r="N36" s="64"/>
+      <c r="O36" s="65"/>
       <c r="P36" s="13">
         <f>P35+P34</f>
         <v>0.19791666666666674</v>
       </c>
-      <c r="Q36" s="73"/>
-      <c r="R36" s="74"/>
+      <c r="Q36" s="59"/>
+      <c r="R36" s="60"/>
       <c r="S36" s="13">
         <f>S35+S34</f>
         <v>0.19791666666666674</v>
       </c>
-      <c r="T36" s="73"/>
-      <c r="U36" s="74"/>
+      <c r="T36" s="59"/>
+      <c r="U36" s="60"/>
       <c r="V36" s="13">
         <f>V35+V34</f>
         <v>0.30208333333333337</v>
@@ -6221,7 +6218,7 @@
     <row r="38" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B39" s="82">
         <v>44025</v>
@@ -6262,7 +6259,7 @@
     </row>
     <row r="40" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B40" s="85"/>
       <c r="C40" s="86"/>
@@ -6288,8 +6285,8 @@
       <c r="W40" s="3"/>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A41" s="77" t="s">
-        <v>7</v>
+      <c r="A41" s="79" t="s">
+        <v>6</v>
       </c>
       <c r="B41" s="49">
         <v>0.32291666666666669</v>
@@ -6348,7 +6345,7 @@
       <c r="W41" s="3"/>
     </row>
     <row r="42" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="78"/>
+      <c r="A42" s="80"/>
       <c r="B42" s="51">
         <v>0.5</v>
       </c>
@@ -6410,45 +6407,45 @@
       <c r="W42" s="3"/>
     </row>
     <row r="43" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="79"/>
-      <c r="B43" s="62"/>
-      <c r="C43" s="63"/>
+      <c r="A43" s="81"/>
+      <c r="B43" s="64"/>
+      <c r="C43" s="65"/>
       <c r="D43" s="13">
         <f>D42+D41</f>
         <v>0.24999999999999994</v>
       </c>
-      <c r="E43" s="62"/>
-      <c r="F43" s="63"/>
+      <c r="E43" s="64"/>
+      <c r="F43" s="65"/>
       <c r="G43" s="13">
         <f>G42+G41</f>
         <v>0.24999999999999994</v>
       </c>
-      <c r="H43" s="62"/>
-      <c r="I43" s="63"/>
+      <c r="H43" s="64"/>
+      <c r="I43" s="65"/>
       <c r="J43" s="13">
         <f>J42+J41</f>
         <v>0</v>
       </c>
-      <c r="K43" s="62"/>
-      <c r="L43" s="63"/>
+      <c r="K43" s="64"/>
+      <c r="L43" s="65"/>
       <c r="M43" s="13">
         <f>M42+M41</f>
         <v>0</v>
       </c>
-      <c r="N43" s="62"/>
-      <c r="O43" s="63"/>
+      <c r="N43" s="64"/>
+      <c r="O43" s="65"/>
       <c r="P43" s="13">
         <f>P42+P41</f>
         <v>0</v>
       </c>
-      <c r="Q43" s="73"/>
-      <c r="R43" s="74"/>
+      <c r="Q43" s="59"/>
+      <c r="R43" s="60"/>
       <c r="S43" s="13">
         <f>S42+S41</f>
         <v>0.41666666666666669</v>
       </c>
-      <c r="T43" s="73"/>
-      <c r="U43" s="74"/>
+      <c r="T43" s="59"/>
+      <c r="U43" s="60"/>
       <c r="V43" s="13">
         <f>V42+V41</f>
         <v>0.29166666666666663</v>
@@ -6459,8 +6456,8 @@
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A44" s="59" t="s">
-        <v>8</v>
+      <c r="A44" s="76" t="s">
+        <v>7</v>
       </c>
       <c r="B44" s="4"/>
       <c r="C44" s="5"/>
@@ -6519,7 +6516,7 @@
       <c r="W44" s="3"/>
     </row>
     <row r="45" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="60"/>
+      <c r="A45" s="77"/>
       <c r="B45" s="8"/>
       <c r="C45" s="9"/>
       <c r="D45" s="10">
@@ -6577,45 +6574,45 @@
       <c r="W45" s="3"/>
     </row>
     <row r="46" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="61"/>
-      <c r="B46" s="62"/>
-      <c r="C46" s="63"/>
+      <c r="A46" s="78"/>
+      <c r="B46" s="64"/>
+      <c r="C46" s="65"/>
       <c r="D46" s="13">
         <f>D45+D44</f>
         <v>0</v>
       </c>
-      <c r="E46" s="62"/>
-      <c r="F46" s="63"/>
+      <c r="E46" s="64"/>
+      <c r="F46" s="65"/>
       <c r="G46" s="13">
         <f>G45+G44</f>
         <v>0.25</v>
       </c>
-      <c r="H46" s="62"/>
-      <c r="I46" s="63"/>
+      <c r="H46" s="64"/>
+      <c r="I46" s="65"/>
       <c r="J46" s="13">
         <f>J45+J44</f>
         <v>0.25</v>
       </c>
-      <c r="K46" s="62"/>
-      <c r="L46" s="63"/>
+      <c r="K46" s="64"/>
+      <c r="L46" s="65"/>
       <c r="M46" s="13">
         <f>M45+M44</f>
         <v>0</v>
       </c>
-      <c r="N46" s="62"/>
-      <c r="O46" s="63"/>
+      <c r="N46" s="64"/>
+      <c r="O46" s="65"/>
       <c r="P46" s="13">
         <f>P45+P44</f>
         <v>0.24999999999999994</v>
       </c>
-      <c r="Q46" s="62"/>
-      <c r="R46" s="63"/>
+      <c r="Q46" s="64"/>
+      <c r="R46" s="65"/>
       <c r="S46" s="13">
         <f>S45+S44</f>
         <v>0</v>
       </c>
-      <c r="T46" s="62"/>
-      <c r="U46" s="63"/>
+      <c r="T46" s="64"/>
+      <c r="U46" s="65"/>
       <c r="V46" s="13">
         <f>V45+V44</f>
         <v>0</v>
@@ -6626,8 +6623,8 @@
       </c>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A47" s="64" t="s">
-        <v>9</v>
+      <c r="A47" s="71" t="s">
+        <v>8</v>
       </c>
       <c r="B47" s="49">
         <v>0.59375</v>
@@ -6683,7 +6680,7 @@
       <c r="W47" s="3"/>
     </row>
     <row r="48" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="65"/>
+      <c r="A48" s="72"/>
       <c r="B48" s="51">
         <v>0.78125</v>
       </c>
@@ -6723,8 +6720,8 @@
         <f>O48-N48</f>
         <v>0</v>
       </c>
-      <c r="Q48" s="75"/>
-      <c r="R48" s="76"/>
+      <c r="Q48" s="69"/>
+      <c r="R48" s="70"/>
       <c r="S48" s="11">
         <v>0</v>
       </c>
@@ -6737,45 +6734,45 @@
       <c r="W48" s="3"/>
     </row>
     <row r="49" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="66"/>
-      <c r="B49" s="62"/>
-      <c r="C49" s="63"/>
+      <c r="A49" s="73"/>
+      <c r="B49" s="64"/>
+      <c r="C49" s="65"/>
       <c r="D49" s="13">
         <f>D47+D48</f>
         <v>0.25</v>
       </c>
-      <c r="E49" s="62"/>
-      <c r="F49" s="63"/>
+      <c r="E49" s="64"/>
+      <c r="F49" s="65"/>
       <c r="G49" s="13">
         <f>G48+G47</f>
         <v>0</v>
       </c>
-      <c r="H49" s="62"/>
-      <c r="I49" s="63"/>
+      <c r="H49" s="64"/>
+      <c r="I49" s="65"/>
       <c r="J49" s="13">
         <f>J48+J47</f>
         <v>0.24999999999999994</v>
       </c>
-      <c r="K49" s="62"/>
-      <c r="L49" s="63"/>
+      <c r="K49" s="64"/>
+      <c r="L49" s="65"/>
       <c r="M49" s="13">
         <f>M48+M47</f>
         <v>0.24999999999999994</v>
       </c>
-      <c r="N49" s="62"/>
-      <c r="O49" s="63"/>
+      <c r="N49" s="64"/>
+      <c r="O49" s="65"/>
       <c r="P49" s="13">
         <f>P48+P47</f>
         <v>0</v>
       </c>
-      <c r="Q49" s="62"/>
-      <c r="R49" s="63"/>
+      <c r="Q49" s="64"/>
+      <c r="R49" s="65"/>
       <c r="S49" s="13">
         <f>S48+S47</f>
         <v>0</v>
       </c>
-      <c r="T49" s="62"/>
-      <c r="U49" s="63"/>
+      <c r="T49" s="64"/>
+      <c r="U49" s="65"/>
       <c r="V49" s="13">
         <f>V48+V47</f>
         <v>0</v>
@@ -6786,8 +6783,8 @@
       </c>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A50" s="90" t="s">
-        <v>10</v>
+      <c r="A50" s="66" t="s">
+        <v>9</v>
       </c>
       <c r="B50" s="4"/>
       <c r="C50" s="5"/>
@@ -6835,7 +6832,7 @@
       <c r="W50" s="3"/>
     </row>
     <row r="51" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="91"/>
+      <c r="A51" s="67"/>
       <c r="B51" s="8"/>
       <c r="C51" s="9"/>
       <c r="D51" s="10">
@@ -6901,45 +6898,45 @@
       <c r="W51" s="3"/>
     </row>
     <row r="52" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="92"/>
-      <c r="B52" s="62"/>
-      <c r="C52" s="63"/>
+      <c r="A52" s="68"/>
+      <c r="B52" s="64"/>
+      <c r="C52" s="65"/>
       <c r="D52" s="13">
         <f>D50+D51</f>
         <v>0</v>
       </c>
-      <c r="E52" s="62"/>
-      <c r="F52" s="63"/>
+      <c r="E52" s="64"/>
+      <c r="F52" s="65"/>
       <c r="G52" s="13">
         <f>G51+G50</f>
         <v>0</v>
       </c>
-      <c r="H52" s="62"/>
-      <c r="I52" s="63"/>
+      <c r="H52" s="64"/>
+      <c r="I52" s="65"/>
       <c r="J52" s="13">
         <f>J51+J50</f>
         <v>0.19791666666666674</v>
       </c>
-      <c r="K52" s="62"/>
-      <c r="L52" s="63"/>
+      <c r="K52" s="64"/>
+      <c r="L52" s="65"/>
       <c r="M52" s="13">
         <f>M51+M50</f>
         <v>0.19791666666666674</v>
       </c>
-      <c r="N52" s="62"/>
-      <c r="O52" s="63"/>
+      <c r="N52" s="64"/>
+      <c r="O52" s="65"/>
       <c r="P52" s="13">
         <f>P51+P50</f>
         <v>0.19791666666666674</v>
       </c>
-      <c r="Q52" s="73"/>
-      <c r="R52" s="74"/>
+      <c r="Q52" s="59"/>
+      <c r="R52" s="60"/>
       <c r="S52" s="13">
         <f>S51+S50</f>
         <v>0.19791666666666674</v>
       </c>
-      <c r="T52" s="73"/>
-      <c r="U52" s="74"/>
+      <c r="T52" s="59"/>
+      <c r="U52" s="60"/>
       <c r="V52" s="13">
         <f>V51+V50</f>
         <v>0.30208333333333337</v>
@@ -6950,8 +6947,8 @@
       </c>
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A53" s="95" t="s">
-        <v>11</v>
+      <c r="A53" s="61" t="s">
+        <v>10</v>
       </c>
       <c r="B53" s="4"/>
       <c r="C53" s="5"/>
@@ -7006,7 +7003,7 @@
       <c r="W53" s="3"/>
     </row>
     <row r="54" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="96"/>
+      <c r="A54" s="62"/>
       <c r="B54" s="55">
         <v>0.60416666666666663</v>
       </c>
@@ -7068,45 +7065,45 @@
       <c r="W54" s="3"/>
     </row>
     <row r="55" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="97"/>
-      <c r="B55" s="62"/>
-      <c r="C55" s="63"/>
+      <c r="A55" s="63"/>
+      <c r="B55" s="64"/>
+      <c r="C55" s="65"/>
       <c r="D55" s="13">
         <f>D54+D53</f>
         <v>0.19791666666666674</v>
       </c>
-      <c r="E55" s="62"/>
-      <c r="F55" s="63"/>
+      <c r="E55" s="64"/>
+      <c r="F55" s="65"/>
       <c r="G55" s="13">
         <f>G53+G54</f>
         <v>0.19791666666666674</v>
       </c>
-      <c r="H55" s="62"/>
-      <c r="I55" s="63"/>
+      <c r="H55" s="64"/>
+      <c r="I55" s="65"/>
       <c r="J55" s="13">
         <f>J53+J54</f>
         <v>0</v>
       </c>
-      <c r="K55" s="62"/>
-      <c r="L55" s="63"/>
+      <c r="K55" s="64"/>
+      <c r="L55" s="65"/>
       <c r="M55" s="13">
         <f>M53+M54</f>
         <v>0.25</v>
       </c>
-      <c r="N55" s="62"/>
-      <c r="O55" s="63"/>
+      <c r="N55" s="64"/>
+      <c r="O55" s="65"/>
       <c r="P55" s="13">
         <f>P53+P54</f>
         <v>0.25</v>
       </c>
-      <c r="Q55" s="73"/>
-      <c r="R55" s="74"/>
+      <c r="Q55" s="59"/>
+      <c r="R55" s="60"/>
       <c r="S55" s="13">
         <f>S54+S53</f>
         <v>0</v>
       </c>
-      <c r="T55" s="73"/>
-      <c r="U55" s="74"/>
+      <c r="T55" s="59"/>
+      <c r="U55" s="60"/>
       <c r="V55" s="13">
         <f>V54+V53</f>
         <v>0</v>
@@ -7119,75 +7116,75 @@
     <row r="57" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="58" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B58" s="67">
+        <v>11</v>
+      </c>
+      <c r="B58" s="88">
         <v>44032</v>
       </c>
-      <c r="C58" s="68"/>
-      <c r="D58" s="69"/>
-      <c r="E58" s="67">
+      <c r="C58" s="89"/>
+      <c r="D58" s="90"/>
+      <c r="E58" s="88">
         <v>44033</v>
       </c>
-      <c r="F58" s="68"/>
-      <c r="G58" s="69"/>
-      <c r="H58" s="67">
+      <c r="F58" s="89"/>
+      <c r="G58" s="90"/>
+      <c r="H58" s="88">
         <v>44034</v>
       </c>
-      <c r="I58" s="68"/>
-      <c r="J58" s="69"/>
-      <c r="K58" s="67">
+      <c r="I58" s="89"/>
+      <c r="J58" s="90"/>
+      <c r="K58" s="88">
         <v>44035</v>
       </c>
-      <c r="L58" s="68"/>
-      <c r="M58" s="69"/>
-      <c r="N58" s="67">
+      <c r="L58" s="89"/>
+      <c r="M58" s="90"/>
+      <c r="N58" s="88">
         <v>44036</v>
       </c>
-      <c r="O58" s="68"/>
-      <c r="P58" s="69"/>
-      <c r="Q58" s="67">
+      <c r="O58" s="89"/>
+      <c r="P58" s="90"/>
+      <c r="Q58" s="88">
         <v>44037</v>
       </c>
-      <c r="R58" s="68"/>
-      <c r="S58" s="69"/>
-      <c r="T58" s="67">
+      <c r="R58" s="89"/>
+      <c r="S58" s="90"/>
+      <c r="T58" s="88">
         <v>44038</v>
       </c>
-      <c r="U58" s="68"/>
-      <c r="V58" s="69"/>
+      <c r="U58" s="89"/>
+      <c r="V58" s="90"/>
       <c r="W58" s="15"/>
     </row>
     <row r="59" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B59" s="70"/>
-      <c r="C59" s="71"/>
-      <c r="D59" s="72"/>
-      <c r="E59" s="70"/>
-      <c r="F59" s="71"/>
-      <c r="G59" s="72"/>
-      <c r="H59" s="70"/>
-      <c r="I59" s="71"/>
-      <c r="J59" s="72"/>
-      <c r="K59" s="70"/>
-      <c r="L59" s="71"/>
-      <c r="M59" s="72"/>
-      <c r="N59" s="70"/>
-      <c r="O59" s="71"/>
-      <c r="P59" s="72"/>
-      <c r="Q59" s="70"/>
-      <c r="R59" s="71"/>
-      <c r="S59" s="72"/>
-      <c r="T59" s="70"/>
-      <c r="U59" s="71"/>
-      <c r="V59" s="72"/>
+        <v>3</v>
+      </c>
+      <c r="B59" s="91"/>
+      <c r="C59" s="92"/>
+      <c r="D59" s="93"/>
+      <c r="E59" s="91"/>
+      <c r="F59" s="92"/>
+      <c r="G59" s="93"/>
+      <c r="H59" s="91"/>
+      <c r="I59" s="92"/>
+      <c r="J59" s="93"/>
+      <c r="K59" s="91"/>
+      <c r="L59" s="92"/>
+      <c r="M59" s="93"/>
+      <c r="N59" s="91"/>
+      <c r="O59" s="92"/>
+      <c r="P59" s="93"/>
+      <c r="Q59" s="91"/>
+      <c r="R59" s="92"/>
+      <c r="S59" s="93"/>
+      <c r="T59" s="91"/>
+      <c r="U59" s="92"/>
+      <c r="V59" s="93"/>
       <c r="W59" s="3"/>
     </row>
     <row r="60" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A60" s="77" t="s">
-        <v>7</v>
+      <c r="A60" s="79" t="s">
+        <v>6</v>
       </c>
       <c r="B60" s="4"/>
       <c r="C60" s="5"/>
@@ -7250,7 +7247,7 @@
       <c r="W60" s="3"/>
     </row>
     <row r="61" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="78"/>
+      <c r="A61" s="80"/>
       <c r="B61" s="8"/>
       <c r="C61" s="9"/>
       <c r="D61" s="10">
@@ -7312,45 +7309,45 @@
       <c r="W61" s="3"/>
     </row>
     <row r="62" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="79"/>
-      <c r="B62" s="62"/>
-      <c r="C62" s="63"/>
+      <c r="A62" s="81"/>
+      <c r="B62" s="64"/>
+      <c r="C62" s="65"/>
       <c r="D62" s="13">
         <f>D61+D60</f>
         <v>0</v>
       </c>
-      <c r="E62" s="62"/>
-      <c r="F62" s="63"/>
+      <c r="E62" s="64"/>
+      <c r="F62" s="65"/>
       <c r="G62" s="13">
         <f>G60+G61</f>
         <v>0.25</v>
       </c>
-      <c r="H62" s="62"/>
-      <c r="I62" s="63"/>
+      <c r="H62" s="64"/>
+      <c r="I62" s="65"/>
       <c r="J62" s="13">
         <f>J60+J61</f>
         <v>0.25</v>
       </c>
-      <c r="K62" s="62"/>
-      <c r="L62" s="63"/>
+      <c r="K62" s="64"/>
+      <c r="L62" s="65"/>
       <c r="M62" s="13">
         <f>M60+M61</f>
         <v>0.25</v>
       </c>
-      <c r="N62" s="62"/>
-      <c r="O62" s="63"/>
+      <c r="N62" s="64"/>
+      <c r="O62" s="65"/>
       <c r="P62" s="13">
         <f>P60+P61</f>
         <v>0.25</v>
       </c>
-      <c r="Q62" s="73"/>
-      <c r="R62" s="74"/>
+      <c r="Q62" s="59"/>
+      <c r="R62" s="60"/>
       <c r="S62" s="13">
         <f>S61+S60</f>
         <v>0</v>
       </c>
-      <c r="T62" s="73"/>
-      <c r="U62" s="74"/>
+      <c r="T62" s="59"/>
+      <c r="U62" s="60"/>
       <c r="V62" s="13">
         <f>V61+V60</f>
         <v>0</v>
@@ -7361,8 +7358,8 @@
       </c>
     </row>
     <row r="63" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A63" s="59" t="s">
-        <v>8</v>
+      <c r="A63" s="76" t="s">
+        <v>7</v>
       </c>
       <c r="B63" s="34"/>
       <c r="C63" s="35"/>
@@ -7409,7 +7406,7 @@
       <c r="W63" s="3"/>
     </row>
     <row r="64" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="60"/>
+      <c r="A64" s="77"/>
       <c r="B64" s="43"/>
       <c r="C64" s="40"/>
       <c r="D64" s="41">
@@ -7455,45 +7452,45 @@
       <c r="W64" s="3"/>
     </row>
     <row r="65" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="61"/>
-      <c r="B65" s="80"/>
-      <c r="C65" s="81"/>
+      <c r="A65" s="78"/>
+      <c r="B65" s="94"/>
+      <c r="C65" s="95"/>
       <c r="D65" s="42">
         <f>D64+D63</f>
         <v>0</v>
       </c>
-      <c r="E65" s="80"/>
-      <c r="F65" s="81"/>
+      <c r="E65" s="94"/>
+      <c r="F65" s="95"/>
       <c r="G65" s="42">
         <f>G64+G63</f>
         <v>0</v>
       </c>
-      <c r="H65" s="80"/>
-      <c r="I65" s="81"/>
+      <c r="H65" s="94"/>
+      <c r="I65" s="95"/>
       <c r="J65" s="42">
         <f>J64+J63</f>
         <v>0</v>
       </c>
-      <c r="K65" s="80"/>
-      <c r="L65" s="81"/>
+      <c r="K65" s="94"/>
+      <c r="L65" s="95"/>
       <c r="M65" s="42">
         <f>M64+M63</f>
         <v>0</v>
       </c>
-      <c r="N65" s="80"/>
-      <c r="O65" s="81"/>
+      <c r="N65" s="94"/>
+      <c r="O65" s="95"/>
       <c r="P65" s="42">
         <f>P64+P63</f>
         <v>0</v>
       </c>
-      <c r="Q65" s="80"/>
-      <c r="R65" s="81"/>
+      <c r="Q65" s="94"/>
+      <c r="R65" s="95"/>
       <c r="S65" s="42">
         <f>S64+S63</f>
         <v>0</v>
       </c>
-      <c r="T65" s="80"/>
-      <c r="U65" s="81"/>
+      <c r="T65" s="94"/>
+      <c r="U65" s="95"/>
       <c r="V65" s="42">
         <f>V64+V63</f>
         <v>0</v>
@@ -7504,8 +7501,8 @@
       </c>
     </row>
     <row r="66" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A66" s="64" t="s">
-        <v>9</v>
+      <c r="A66" s="71" t="s">
+        <v>8</v>
       </c>
       <c r="B66" s="49">
         <v>0.32291666666666669</v>
@@ -7564,7 +7561,7 @@
       <c r="W66" s="3"/>
     </row>
     <row r="67" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="65"/>
+      <c r="A67" s="72"/>
       <c r="B67" s="51">
         <v>0.5</v>
       </c>
@@ -7626,45 +7623,45 @@
       <c r="W67" s="3"/>
     </row>
     <row r="68" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="66"/>
-      <c r="B68" s="62"/>
-      <c r="C68" s="63"/>
+      <c r="A68" s="73"/>
+      <c r="B68" s="64"/>
+      <c r="C68" s="65"/>
       <c r="D68" s="13">
         <f>D67+D66</f>
         <v>0.24999999999999994</v>
       </c>
-      <c r="E68" s="62"/>
-      <c r="F68" s="63"/>
+      <c r="E68" s="64"/>
+      <c r="F68" s="65"/>
       <c r="G68" s="13">
         <f>G67+G66</f>
         <v>0.24999999999999994</v>
       </c>
-      <c r="H68" s="62"/>
-      <c r="I68" s="63"/>
+      <c r="H68" s="64"/>
+      <c r="I68" s="65"/>
       <c r="J68" s="13">
         <f>J67+J66</f>
         <v>0</v>
       </c>
-      <c r="K68" s="62"/>
-      <c r="L68" s="63"/>
+      <c r="K68" s="64"/>
+      <c r="L68" s="65"/>
       <c r="M68" s="13">
         <f>M67+M66</f>
         <v>0</v>
       </c>
-      <c r="N68" s="62"/>
-      <c r="O68" s="63"/>
+      <c r="N68" s="64"/>
+      <c r="O68" s="65"/>
       <c r="P68" s="13">
         <f>P67+P66</f>
         <v>0</v>
       </c>
-      <c r="Q68" s="73"/>
-      <c r="R68" s="74"/>
+      <c r="Q68" s="59"/>
+      <c r="R68" s="60"/>
       <c r="S68" s="13">
         <f>S67+S66</f>
         <v>0.41666666666666669</v>
       </c>
-      <c r="T68" s="73"/>
-      <c r="U68" s="74"/>
+      <c r="T68" s="59"/>
+      <c r="U68" s="60"/>
       <c r="V68" s="13">
         <f>V67+V66</f>
         <v>0.29166666666666663</v>
@@ -7675,8 +7672,8 @@
       </c>
     </row>
     <row r="69" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A69" s="90" t="s">
-        <v>10</v>
+      <c r="A69" s="66" t="s">
+        <v>9</v>
       </c>
       <c r="B69" s="4"/>
       <c r="C69" s="5"/>
@@ -7724,7 +7721,7 @@
       <c r="W69" s="3"/>
     </row>
     <row r="70" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="91"/>
+      <c r="A70" s="67"/>
       <c r="B70" s="55">
         <v>0.60416666666666663</v>
       </c>
@@ -7794,45 +7791,45 @@
       <c r="W70" s="3"/>
     </row>
     <row r="71" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="92"/>
-      <c r="B71" s="62"/>
-      <c r="C71" s="63"/>
+      <c r="A71" s="68"/>
+      <c r="B71" s="64"/>
+      <c r="C71" s="65"/>
       <c r="D71" s="13">
         <f>D69+D70</f>
         <v>0.19791666666666674</v>
       </c>
-      <c r="E71" s="62"/>
-      <c r="F71" s="63"/>
+      <c r="E71" s="64"/>
+      <c r="F71" s="65"/>
       <c r="G71" s="13">
         <f>G70+G69</f>
         <v>0</v>
       </c>
-      <c r="H71" s="62"/>
-      <c r="I71" s="63"/>
+      <c r="H71" s="64"/>
+      <c r="I71" s="65"/>
       <c r="J71" s="13">
         <f>J70+J69</f>
         <v>0.19791666666666674</v>
       </c>
-      <c r="K71" s="62"/>
-      <c r="L71" s="63"/>
+      <c r="K71" s="64"/>
+      <c r="L71" s="65"/>
       <c r="M71" s="13">
         <f>M70+M69</f>
         <v>0.19791666666666674</v>
       </c>
-      <c r="N71" s="62"/>
-      <c r="O71" s="63"/>
+      <c r="N71" s="64"/>
+      <c r="O71" s="65"/>
       <c r="P71" s="13">
         <f>P70+P69</f>
         <v>0.19791666666666674</v>
       </c>
-      <c r="Q71" s="73"/>
-      <c r="R71" s="74"/>
+      <c r="Q71" s="59"/>
+      <c r="R71" s="60"/>
       <c r="S71" s="13">
         <f>S70+S69</f>
         <v>0.19791666666666674</v>
       </c>
-      <c r="T71" s="73"/>
-      <c r="U71" s="74"/>
+      <c r="T71" s="59"/>
+      <c r="U71" s="60"/>
       <c r="V71" s="13">
         <f>V70+V69</f>
         <v>0.30208333333333337</v>
@@ -7843,8 +7840,8 @@
       </c>
     </row>
     <row r="72" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A72" s="95" t="s">
-        <v>11</v>
+      <c r="A72" s="61" t="s">
+        <v>10</v>
       </c>
       <c r="B72" s="49">
         <v>0.59375</v>
@@ -7904,7 +7901,7 @@
       <c r="W72" s="3"/>
     </row>
     <row r="73" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="96"/>
+      <c r="A73" s="62"/>
       <c r="B73" s="51">
         <v>0.78125</v>
       </c>
@@ -7952,8 +7949,8 @@
         <f>O73-N73</f>
         <v>0.10416666666666663</v>
       </c>
-      <c r="Q73" s="75"/>
-      <c r="R73" s="76"/>
+      <c r="Q73" s="69"/>
+      <c r="R73" s="70"/>
       <c r="S73" s="11">
         <v>0</v>
       </c>
@@ -7966,45 +7963,45 @@
       <c r="W73" s="3"/>
     </row>
     <row r="74" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="97"/>
-      <c r="B74" s="62"/>
-      <c r="C74" s="63"/>
+      <c r="A74" s="63"/>
+      <c r="B74" s="64"/>
+      <c r="C74" s="65"/>
       <c r="D74" s="13">
         <f>D72+D73</f>
         <v>0.25</v>
       </c>
-      <c r="E74" s="62"/>
-      <c r="F74" s="63"/>
+      <c r="E74" s="64"/>
+      <c r="F74" s="65"/>
       <c r="G74" s="13">
         <f>G73+G72</f>
         <v>0</v>
       </c>
-      <c r="H74" s="62"/>
-      <c r="I74" s="63"/>
+      <c r="H74" s="64"/>
+      <c r="I74" s="65"/>
       <c r="J74" s="13">
         <f>J73+J72</f>
         <v>0.24999999999999994</v>
       </c>
-      <c r="K74" s="62"/>
-      <c r="L74" s="63"/>
+      <c r="K74" s="64"/>
+      <c r="L74" s="65"/>
       <c r="M74" s="13">
         <f>M73+M72</f>
         <v>0.24999999999999994</v>
       </c>
-      <c r="N74" s="62"/>
-      <c r="O74" s="63"/>
+      <c r="N74" s="64"/>
+      <c r="O74" s="65"/>
       <c r="P74" s="13">
         <f>P73+P72</f>
         <v>0.24999999999999994</v>
       </c>
-      <c r="Q74" s="62"/>
-      <c r="R74" s="63"/>
+      <c r="Q74" s="64"/>
+      <c r="R74" s="65"/>
       <c r="S74" s="13">
         <f>S73+S72</f>
         <v>0</v>
       </c>
-      <c r="T74" s="62"/>
-      <c r="U74" s="63"/>
+      <c r="T74" s="64"/>
+      <c r="U74" s="65"/>
       <c r="V74" s="13">
         <f>V73+V72</f>
         <v>0</v>
@@ -8017,7 +8014,7 @@
     <row r="76" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="77" spans="1:23" ht="14" x14ac:dyDescent="0.15">
       <c r="A77" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B77" s="82">
         <v>44039</v>
@@ -8058,7 +8055,7 @@
     </row>
     <row r="78" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B78" s="85"/>
       <c r="C78" s="86"/>
@@ -8084,8 +8081,8 @@
       <c r="W78" s="3"/>
     </row>
     <row r="79" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A79" s="77" t="s">
-        <v>7</v>
+      <c r="A79" s="79" t="s">
+        <v>6</v>
       </c>
       <c r="B79" s="49">
         <v>0.59375</v>
@@ -8145,7 +8142,7 @@
       <c r="W79" s="3"/>
     </row>
     <row r="80" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="78"/>
+      <c r="A80" s="80"/>
       <c r="B80" s="51">
         <v>0.78125</v>
       </c>
@@ -8189,8 +8186,8 @@
         <f>O80-N80</f>
         <v>0.10416666666666663</v>
       </c>
-      <c r="Q80" s="75"/>
-      <c r="R80" s="76"/>
+      <c r="Q80" s="69"/>
+      <c r="R80" s="70"/>
       <c r="S80" s="11">
         <v>0</v>
       </c>
@@ -8203,45 +8200,45 @@
       <c r="W80" s="3"/>
     </row>
     <row r="81" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="79"/>
-      <c r="B81" s="62"/>
-      <c r="C81" s="63"/>
+      <c r="A81" s="81"/>
+      <c r="B81" s="64"/>
+      <c r="C81" s="65"/>
       <c r="D81" s="13">
         <f>D79+D80</f>
         <v>0.25</v>
       </c>
-      <c r="E81" s="62"/>
-      <c r="F81" s="63"/>
+      <c r="E81" s="64"/>
+      <c r="F81" s="65"/>
       <c r="G81" s="13">
         <f>G80+G79</f>
         <v>0</v>
       </c>
-      <c r="H81" s="62"/>
-      <c r="I81" s="63"/>
+      <c r="H81" s="64"/>
+      <c r="I81" s="65"/>
       <c r="J81" s="13">
         <f>J80+J79</f>
         <v>0.24999999999999994</v>
       </c>
-      <c r="K81" s="62"/>
-      <c r="L81" s="63"/>
+      <c r="K81" s="64"/>
+      <c r="L81" s="65"/>
       <c r="M81" s="13">
         <f>M80+M79</f>
         <v>0.24999999999999994</v>
       </c>
-      <c r="N81" s="62"/>
-      <c r="O81" s="63"/>
+      <c r="N81" s="64"/>
+      <c r="O81" s="65"/>
       <c r="P81" s="13">
         <f>P80+P79</f>
         <v>0.24999999999999994</v>
       </c>
-      <c r="Q81" s="62"/>
-      <c r="R81" s="63"/>
+      <c r="Q81" s="64"/>
+      <c r="R81" s="65"/>
       <c r="S81" s="13">
         <f>S80+S79</f>
         <v>0</v>
       </c>
-      <c r="T81" s="62"/>
-      <c r="U81" s="63"/>
+      <c r="T81" s="64"/>
+      <c r="U81" s="65"/>
       <c r="V81" s="13">
         <f>V80+V79</f>
         <v>0</v>
@@ -8252,8 +8249,8 @@
       </c>
     </row>
     <row r="82" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A82" s="59" t="s">
-        <v>8</v>
+      <c r="A82" s="76" t="s">
+        <v>7</v>
       </c>
       <c r="B82" s="49">
         <v>0.32291666666666669</v>
@@ -8312,7 +8309,7 @@
       <c r="W82" s="3"/>
     </row>
     <row r="83" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="60"/>
+      <c r="A83" s="77"/>
       <c r="B83" s="51">
         <v>0.5</v>
       </c>
@@ -8374,45 +8371,45 @@
       <c r="W83" s="3"/>
     </row>
     <row r="84" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="61"/>
-      <c r="B84" s="62"/>
-      <c r="C84" s="63"/>
+      <c r="A84" s="78"/>
+      <c r="B84" s="64"/>
+      <c r="C84" s="65"/>
       <c r="D84" s="13">
         <f>D83+D82</f>
         <v>0.24999999999999994</v>
       </c>
-      <c r="E84" s="62"/>
-      <c r="F84" s="63"/>
+      <c r="E84" s="64"/>
+      <c r="F84" s="65"/>
       <c r="G84" s="13">
         <f>G83+G82</f>
         <v>0.24999999999999994</v>
       </c>
-      <c r="H84" s="62"/>
-      <c r="I84" s="63"/>
+      <c r="H84" s="64"/>
+      <c r="I84" s="65"/>
       <c r="J84" s="13">
         <f>J83+J82</f>
         <v>0</v>
       </c>
-      <c r="K84" s="62"/>
-      <c r="L84" s="63"/>
+      <c r="K84" s="64"/>
+      <c r="L84" s="65"/>
       <c r="M84" s="13">
         <f>M83+M82</f>
         <v>0</v>
       </c>
-      <c r="N84" s="62"/>
-      <c r="O84" s="63"/>
+      <c r="N84" s="64"/>
+      <c r="O84" s="65"/>
       <c r="P84" s="13">
         <f>P83+P82</f>
         <v>0</v>
       </c>
-      <c r="Q84" s="73"/>
-      <c r="R84" s="74"/>
+      <c r="Q84" s="59"/>
+      <c r="R84" s="60"/>
       <c r="S84" s="13">
         <f>S83+S82</f>
         <v>0.41666666666666669</v>
       </c>
-      <c r="T84" s="73"/>
-      <c r="U84" s="74"/>
+      <c r="T84" s="59"/>
+      <c r="U84" s="60"/>
       <c r="V84" s="13">
         <f>V83+V82</f>
         <v>0.29166666666666663</v>
@@ -8423,8 +8420,8 @@
       </c>
     </row>
     <row r="85" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A85" s="64" t="s">
-        <v>9</v>
+      <c r="A85" s="71" t="s">
+        <v>8</v>
       </c>
       <c r="B85" s="4"/>
       <c r="C85" s="5"/>
@@ -8483,7 +8480,7 @@
       <c r="W85" s="3"/>
     </row>
     <row r="86" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="65"/>
+      <c r="A86" s="72"/>
       <c r="B86" s="8"/>
       <c r="C86" s="9"/>
       <c r="D86" s="10">
@@ -8541,45 +8538,45 @@
       <c r="W86" s="3"/>
     </row>
     <row r="87" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="66"/>
-      <c r="B87" s="62"/>
-      <c r="C87" s="63"/>
+      <c r="A87" s="73"/>
+      <c r="B87" s="64"/>
+      <c r="C87" s="65"/>
       <c r="D87" s="13">
         <f>D86+D85</f>
         <v>0</v>
       </c>
-      <c r="E87" s="62"/>
-      <c r="F87" s="63"/>
+      <c r="E87" s="64"/>
+      <c r="F87" s="65"/>
       <c r="G87" s="13">
         <f>G85+G86</f>
         <v>0.25</v>
       </c>
-      <c r="H87" s="62"/>
-      <c r="I87" s="63"/>
+      <c r="H87" s="64"/>
+      <c r="I87" s="65"/>
       <c r="J87" s="13">
         <f>J85+J86</f>
         <v>0.25</v>
       </c>
-      <c r="K87" s="62"/>
-      <c r="L87" s="63"/>
+      <c r="K87" s="64"/>
+      <c r="L87" s="65"/>
       <c r="M87" s="13">
         <f>M85+M86</f>
         <v>0.25</v>
       </c>
-      <c r="N87" s="62"/>
-      <c r="O87" s="63"/>
+      <c r="N87" s="64"/>
+      <c r="O87" s="65"/>
       <c r="P87" s="13">
         <f>P86+P85</f>
         <v>0</v>
       </c>
-      <c r="Q87" s="62"/>
-      <c r="R87" s="63"/>
+      <c r="Q87" s="64"/>
+      <c r="R87" s="65"/>
       <c r="S87" s="13">
         <f>S86+S85</f>
         <v>0</v>
       </c>
-      <c r="T87" s="62"/>
-      <c r="U87" s="63"/>
+      <c r="T87" s="64"/>
+      <c r="U87" s="65"/>
       <c r="V87" s="13">
         <f>V86+V85</f>
         <v>0</v>
@@ -8590,8 +8587,8 @@
       </c>
     </row>
     <row r="88" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A88" s="90" t="s">
-        <v>10</v>
+      <c r="A88" s="66" t="s">
+        <v>9</v>
       </c>
       <c r="B88" s="4"/>
       <c r="C88" s="5"/>
@@ -8638,7 +8635,7 @@
       <c r="W88" s="3"/>
     </row>
     <row r="89" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="91"/>
+      <c r="A89" s="67"/>
       <c r="B89" s="8"/>
       <c r="C89" s="9"/>
       <c r="D89" s="10">
@@ -8696,45 +8693,45 @@
       <c r="W89" s="3"/>
     </row>
     <row r="90" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="92"/>
-      <c r="B90" s="62"/>
-      <c r="C90" s="63"/>
+      <c r="A90" s="68"/>
+      <c r="B90" s="64"/>
+      <c r="C90" s="65"/>
       <c r="D90" s="13">
         <f>D89+D88</f>
         <v>0</v>
       </c>
-      <c r="E90" s="62"/>
-      <c r="F90" s="63"/>
+      <c r="E90" s="64"/>
+      <c r="F90" s="65"/>
       <c r="G90" s="13">
         <f>G88+G89</f>
         <v>0</v>
       </c>
-      <c r="H90" s="62"/>
-      <c r="I90" s="63"/>
+      <c r="H90" s="64"/>
+      <c r="I90" s="65"/>
       <c r="J90" s="13">
         <f>J89+J88</f>
         <v>0.19791666666666674</v>
       </c>
-      <c r="K90" s="62"/>
-      <c r="L90" s="63"/>
+      <c r="K90" s="64"/>
+      <c r="L90" s="65"/>
       <c r="M90" s="13">
         <f>M89+M88</f>
         <v>0.19791666666666674</v>
       </c>
-      <c r="N90" s="62"/>
-      <c r="O90" s="63"/>
+      <c r="N90" s="64"/>
+      <c r="O90" s="65"/>
       <c r="P90" s="13">
         <f>P88+P89</f>
         <v>0.19791666666666674</v>
       </c>
-      <c r="Q90" s="73"/>
-      <c r="R90" s="74"/>
+      <c r="Q90" s="59"/>
+      <c r="R90" s="60"/>
       <c r="S90" s="13">
         <f>S89+S88</f>
         <v>0</v>
       </c>
-      <c r="T90" s="73"/>
-      <c r="U90" s="74"/>
+      <c r="T90" s="59"/>
+      <c r="U90" s="60"/>
       <c r="V90" s="13">
         <f>V89+V88</f>
         <v>0</v>
@@ -8745,8 +8742,8 @@
       </c>
     </row>
     <row r="91" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A91" s="95" t="s">
-        <v>11</v>
+      <c r="A91" s="61" t="s">
+        <v>10</v>
       </c>
       <c r="B91" s="4"/>
       <c r="C91" s="5"/>
@@ -8794,7 +8791,7 @@
       <c r="W91" s="3"/>
     </row>
     <row r="92" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="96"/>
+      <c r="A92" s="62"/>
       <c r="B92" s="55">
         <v>0.60416666666666663</v>
       </c>
@@ -8856,45 +8853,45 @@
       <c r="W92" s="3"/>
     </row>
     <row r="93" spans="1:23" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="97"/>
-      <c r="B93" s="62"/>
-      <c r="C93" s="63"/>
+      <c r="A93" s="63"/>
+      <c r="B93" s="64"/>
+      <c r="C93" s="65"/>
       <c r="D93" s="13">
         <f>D91+D92</f>
         <v>0.19791666666666674</v>
       </c>
-      <c r="E93" s="62"/>
-      <c r="F93" s="63"/>
+      <c r="E93" s="64"/>
+      <c r="F93" s="65"/>
       <c r="G93" s="13">
         <f>G92+G91</f>
         <v>0.19791666666666674</v>
       </c>
-      <c r="H93" s="62"/>
-      <c r="I93" s="63"/>
+      <c r="H93" s="64"/>
+      <c r="I93" s="65"/>
       <c r="J93" s="13">
         <f>J92+J91</f>
         <v>0</v>
       </c>
-      <c r="K93" s="62"/>
-      <c r="L93" s="63"/>
+      <c r="K93" s="64"/>
+      <c r="L93" s="65"/>
       <c r="M93" s="13">
         <f>M92+M91</f>
         <v>0</v>
       </c>
-      <c r="N93" s="62"/>
-      <c r="O93" s="63"/>
+      <c r="N93" s="64"/>
+      <c r="O93" s="65"/>
       <c r="P93" s="13">
         <f>P92+P91</f>
         <v>0</v>
       </c>
-      <c r="Q93" s="73"/>
-      <c r="R93" s="74"/>
+      <c r="Q93" s="59"/>
+      <c r="R93" s="60"/>
       <c r="S93" s="13">
         <f>S92+S91</f>
         <v>0.19791666666666674</v>
       </c>
-      <c r="T93" s="73"/>
-      <c r="U93" s="74"/>
+      <c r="T93" s="59"/>
+      <c r="U93" s="60"/>
       <c r="V93" s="13">
         <f>V92+V91</f>
         <v>0.30208333333333337</v>
@@ -8906,6 +8903,222 @@
     </row>
   </sheetData>
   <mergeCells count="240">
+    <mergeCell ref="N1:P2"/>
+    <mergeCell ref="Q1:S2"/>
+    <mergeCell ref="T1:V2"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="K20:M21"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="B1:D2"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="T11:U11"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="E1:G2"/>
+    <mergeCell ref="T8:U8"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H1:J2"/>
+    <mergeCell ref="K1:M2"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="N20:P21"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="Q20:S21"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="E39:G40"/>
+    <mergeCell ref="H39:J40"/>
+    <mergeCell ref="K39:M40"/>
+    <mergeCell ref="N39:P40"/>
+    <mergeCell ref="Q39:S40"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="T39:V40"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="T27:U27"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="Q58:S59"/>
+    <mergeCell ref="T46:U46"/>
+    <mergeCell ref="T49:U49"/>
+    <mergeCell ref="T58:V59"/>
+    <mergeCell ref="T52:U52"/>
+    <mergeCell ref="Q55:R55"/>
+    <mergeCell ref="Q43:R43"/>
+    <mergeCell ref="T43:U43"/>
+    <mergeCell ref="B39:D40"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="K46:L46"/>
+    <mergeCell ref="N46:O46"/>
+    <mergeCell ref="Q46:R46"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="K43:L43"/>
+    <mergeCell ref="N43:O43"/>
+    <mergeCell ref="A79:A81"/>
+    <mergeCell ref="Q80:R80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="E81:F81"/>
+    <mergeCell ref="H81:I81"/>
+    <mergeCell ref="K81:L81"/>
+    <mergeCell ref="N81:O81"/>
+    <mergeCell ref="Q81:R81"/>
+    <mergeCell ref="Q68:R68"/>
+    <mergeCell ref="B77:D78"/>
+    <mergeCell ref="E77:G78"/>
+    <mergeCell ref="H77:J78"/>
+    <mergeCell ref="K77:M78"/>
+    <mergeCell ref="N77:P78"/>
+    <mergeCell ref="Q77:S78"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="E68:F68"/>
+    <mergeCell ref="H68:I68"/>
+    <mergeCell ref="K68:L68"/>
+    <mergeCell ref="N68:O68"/>
+    <mergeCell ref="Q73:R73"/>
+    <mergeCell ref="N87:O87"/>
+    <mergeCell ref="A82:A84"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="E84:F84"/>
+    <mergeCell ref="H84:I84"/>
+    <mergeCell ref="K84:L84"/>
+    <mergeCell ref="N84:O84"/>
+    <mergeCell ref="Q84:R84"/>
+    <mergeCell ref="T84:U84"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="T14:U14"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="T81:U81"/>
+    <mergeCell ref="T68:U68"/>
+    <mergeCell ref="T77:V78"/>
+    <mergeCell ref="Q62:R62"/>
+    <mergeCell ref="T62:U62"/>
+    <mergeCell ref="B58:D59"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="E65:F65"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="K65:L65"/>
+    <mergeCell ref="N65:O65"/>
+    <mergeCell ref="Q65:R65"/>
+    <mergeCell ref="T65:U65"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="T17:U17"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="T33:U33"/>
+    <mergeCell ref="T30:U30"/>
+    <mergeCell ref="T20:V21"/>
+    <mergeCell ref="T24:U24"/>
+    <mergeCell ref="B20:D21"/>
+    <mergeCell ref="E20:G21"/>
+    <mergeCell ref="H20:J21"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="T36:U36"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="K52:L52"/>
+    <mergeCell ref="N52:O52"/>
+    <mergeCell ref="Q52:R52"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="N55:O55"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="T55:U55"/>
+    <mergeCell ref="Q48:R48"/>
+    <mergeCell ref="K49:L49"/>
+    <mergeCell ref="N49:O49"/>
+    <mergeCell ref="Q49:R49"/>
+    <mergeCell ref="Q71:R71"/>
+    <mergeCell ref="T71:U71"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="A72:A74"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="E74:F74"/>
+    <mergeCell ref="H74:I74"/>
+    <mergeCell ref="K74:L74"/>
+    <mergeCell ref="N74:O74"/>
+    <mergeCell ref="Q74:R74"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="E71:F71"/>
+    <mergeCell ref="H71:I71"/>
+    <mergeCell ref="K71:L71"/>
+    <mergeCell ref="N71:O71"/>
+    <mergeCell ref="A63:A65"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="K62:L62"/>
+    <mergeCell ref="N62:O62"/>
+    <mergeCell ref="E58:G59"/>
+    <mergeCell ref="H58:J59"/>
+    <mergeCell ref="K58:M59"/>
+    <mergeCell ref="N58:P59"/>
     <mergeCell ref="Q93:R93"/>
     <mergeCell ref="T93:U93"/>
     <mergeCell ref="A91:A93"/>
@@ -8924,228 +9137,12 @@
     <mergeCell ref="Q90:R90"/>
     <mergeCell ref="T90:U90"/>
     <mergeCell ref="Q87:R87"/>
-    <mergeCell ref="Q71:R71"/>
-    <mergeCell ref="T71:U71"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="A72:A74"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="E74:F74"/>
-    <mergeCell ref="H74:I74"/>
-    <mergeCell ref="K74:L74"/>
-    <mergeCell ref="N74:O74"/>
-    <mergeCell ref="Q74:R74"/>
-    <mergeCell ref="A69:A71"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="E71:F71"/>
-    <mergeCell ref="H71:I71"/>
-    <mergeCell ref="K71:L71"/>
-    <mergeCell ref="N71:O71"/>
-    <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="T55:U55"/>
-    <mergeCell ref="Q48:R48"/>
-    <mergeCell ref="K49:L49"/>
-    <mergeCell ref="N49:O49"/>
-    <mergeCell ref="Q49:R49"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="N55:O55"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="Q30:R30"/>
-    <mergeCell ref="T36:U36"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="K52:L52"/>
-    <mergeCell ref="N52:O52"/>
-    <mergeCell ref="Q52:R52"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N36:O36"/>
-    <mergeCell ref="T17:U17"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="N33:O33"/>
-    <mergeCell ref="Q33:R33"/>
-    <mergeCell ref="T33:U33"/>
     <mergeCell ref="T87:U87"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="T14:U14"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="T81:U81"/>
     <mergeCell ref="A85:A87"/>
     <mergeCell ref="B87:C87"/>
     <mergeCell ref="E87:F87"/>
     <mergeCell ref="H87:I87"/>
     <mergeCell ref="K87:L87"/>
-    <mergeCell ref="N87:O87"/>
-    <mergeCell ref="A82:A84"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="E84:F84"/>
-    <mergeCell ref="H84:I84"/>
-    <mergeCell ref="K84:L84"/>
-    <mergeCell ref="N84:O84"/>
-    <mergeCell ref="Q84:R84"/>
-    <mergeCell ref="T84:U84"/>
-    <mergeCell ref="A79:A81"/>
-    <mergeCell ref="Q80:R80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="E81:F81"/>
-    <mergeCell ref="H81:I81"/>
-    <mergeCell ref="K81:L81"/>
-    <mergeCell ref="N81:O81"/>
-    <mergeCell ref="Q81:R81"/>
-    <mergeCell ref="Q68:R68"/>
-    <mergeCell ref="T68:U68"/>
-    <mergeCell ref="A63:A65"/>
-    <mergeCell ref="B77:D78"/>
-    <mergeCell ref="E77:G78"/>
-    <mergeCell ref="H77:J78"/>
-    <mergeCell ref="K77:M78"/>
-    <mergeCell ref="N77:P78"/>
-    <mergeCell ref="Q77:S78"/>
-    <mergeCell ref="T77:V78"/>
-    <mergeCell ref="A66:A68"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="E68:F68"/>
-    <mergeCell ref="H68:I68"/>
-    <mergeCell ref="K68:L68"/>
-    <mergeCell ref="N68:O68"/>
-    <mergeCell ref="Q62:R62"/>
-    <mergeCell ref="T62:U62"/>
-    <mergeCell ref="B58:D59"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="E65:F65"/>
-    <mergeCell ref="H65:I65"/>
-    <mergeCell ref="K65:L65"/>
-    <mergeCell ref="N65:O65"/>
-    <mergeCell ref="Q65:R65"/>
-    <mergeCell ref="T65:U65"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="K62:L62"/>
-    <mergeCell ref="N62:O62"/>
-    <mergeCell ref="E58:G59"/>
-    <mergeCell ref="H58:J59"/>
-    <mergeCell ref="K58:M59"/>
-    <mergeCell ref="N58:P59"/>
-    <mergeCell ref="Q58:S59"/>
-    <mergeCell ref="T46:U46"/>
-    <mergeCell ref="T49:U49"/>
-    <mergeCell ref="T58:V59"/>
-    <mergeCell ref="T52:U52"/>
-    <mergeCell ref="Q55:R55"/>
-    <mergeCell ref="Q43:R43"/>
-    <mergeCell ref="T43:U43"/>
-    <mergeCell ref="B39:D40"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="K46:L46"/>
-    <mergeCell ref="N46:O46"/>
-    <mergeCell ref="Q46:R46"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="K43:L43"/>
-    <mergeCell ref="N43:O43"/>
-    <mergeCell ref="T30:U30"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="E39:G40"/>
-    <mergeCell ref="H39:J40"/>
-    <mergeCell ref="K39:M40"/>
-    <mergeCell ref="N39:P40"/>
-    <mergeCell ref="Q39:S40"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="T39:V40"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="T20:V21"/>
-    <mergeCell ref="T24:U24"/>
-    <mergeCell ref="B20:D21"/>
-    <mergeCell ref="E20:G21"/>
-    <mergeCell ref="H20:J21"/>
-    <mergeCell ref="T27:U27"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="N20:P21"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="Q20:S21"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="B1:D2"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="T11:U11"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="E1:G2"/>
-    <mergeCell ref="T8:U8"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H1:J2"/>
-    <mergeCell ref="K1:M2"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="Q73:R73"/>
-    <mergeCell ref="N1:P2"/>
-    <mergeCell ref="Q1:S2"/>
-    <mergeCell ref="T1:V2"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="K20:M21"/>
   </mergeCells>
   <conditionalFormatting sqref="N11:O11">
     <cfRule type="cellIs" dxfId="449" priority="862" operator="equal">

</xml_diff>